<commit_message>
benerin sweetallert di delete koordinat sama template excel
</commit_message>
<xml_diff>
--- a/public/asset/template/template_excel.xlsx
+++ b/public/asset/template/template_excel.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUF\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboard_pju\public\asset\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{643D968C-393B-4A69-87C8-88EEFE9515B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3587DACB-B05C-40E7-962C-C5991A8A26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bro tolong implementasiin ke sc" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Latitude</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>106.815949</t>
+  </si>
+  <si>
+    <t>106.813574</t>
+  </si>
+  <si>
+    <t>-6.358211</t>
+  </si>
+  <si>
+    <t>-6.375125</t>
+  </si>
+  <si>
+    <t>P3</t>
   </si>
 </sst>
 </file>
@@ -97,6 +112,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -123,7 +139,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,15 +354,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884A90F2-AECA-4DB2-A9EA-C6F917B67748}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -378,11 +393,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>-6358211</v>
-      </c>
-      <c r="B2" s="2">
-        <v>106815949</v>
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -402,16 +417,16 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1">
-        <v>5000</v>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>-6375125</v>
-      </c>
-      <c r="B3" s="2">
-        <v>106813574</v>
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -431,15 +446,15 @@
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1">
-        <v>15000</v>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">

</xml_diff>

<commit_message>
menambahkan nama foto di template excel
</commit_message>
<xml_diff>
--- a/public/asset/template/template_excel.xlsx
+++ b/public/asset/template/template_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboard_pju\public\asset\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3587DACB-B05C-40E7-962C-C5991A8A26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8BD8AA-3770-4FCF-9B21-17F0F0ACDD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Latitude</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>Nama Photo</t>
   </si>
 </sst>
 </file>
@@ -355,15 +358,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884A90F2-AECA-4DB2-A9EA-C6F917B67748}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -383,16 +386,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -411,17 +417,18 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -440,17 +447,18 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -469,13 +477,14 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>